<commit_message>
complete spreadsheet of EUL images and BL text
</commit_message>
<xml_diff>
--- a/documentation/Digital Derricke Spreadsheet.xlsx
+++ b/documentation/Digital Derricke Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="279">
   <si>
     <t>File Name</t>
   </si>
@@ -36,108 +36,72 @@
     <t>PL1F1</t>
   </si>
   <si>
-    <t>Plate 1</t>
-  </si>
-  <si>
     <t>EUL_plate02</t>
   </si>
   <si>
     <t>PL2F2</t>
   </si>
   <si>
-    <t>Plate 2</t>
-  </si>
-  <si>
     <t>EUL_plate03</t>
   </si>
   <si>
     <t>PL3F3</t>
   </si>
   <si>
-    <t>Plate 3</t>
-  </si>
-  <si>
     <t>EUL_plate04</t>
   </si>
   <si>
     <t>PL4F4</t>
   </si>
   <si>
-    <t>Plate 4</t>
-  </si>
-  <si>
     <t>EUL_plate05</t>
   </si>
   <si>
     <t>PL5F5</t>
   </si>
   <si>
-    <t>Plate 5</t>
-  </si>
-  <si>
     <t>EUL_plate06</t>
   </si>
   <si>
     <t>PL6F6</t>
   </si>
   <si>
-    <t>Plate 6</t>
-  </si>
-  <si>
     <t>EUL_plate07</t>
   </si>
   <si>
     <t>PL7F7</t>
   </si>
   <si>
-    <t>Plate 7</t>
-  </si>
-  <si>
     <t>EUL_plate08</t>
   </si>
   <si>
     <t>PL8F8</t>
   </si>
   <si>
-    <t>Plate 8</t>
-  </si>
-  <si>
     <t>EUL_plate09</t>
   </si>
   <si>
     <t>PL9F9</t>
   </si>
   <si>
-    <t>Plate 9</t>
-  </si>
-  <si>
     <t>EUL_plate10</t>
   </si>
   <si>
     <t>PL10F10</t>
   </si>
   <si>
-    <t>Plate 10</t>
-  </si>
-  <si>
     <t>EUL_plate11</t>
   </si>
   <si>
     <t>PL11F11</t>
   </si>
   <si>
-    <t>Plate 11</t>
-  </si>
-  <si>
     <t>EUL_plate12</t>
   </si>
   <si>
     <t>PL12F12</t>
   </si>
   <si>
-    <t>Plate 12</t>
-  </si>
-  <si>
     <t>BL001</t>
   </si>
   <si>
@@ -153,9 +117,6 @@
     <t>FMPG1F14</t>
   </si>
   <si>
-    <t>Image of Phillip Sidney (1586); posthumous</t>
-  </si>
-  <si>
     <t>BL003</t>
   </si>
   <si>
@@ -604,6 +565,297 @@
   </si>
   <si>
     <t>BL099</t>
+  </si>
+  <si>
+    <t>PXPG1F61</t>
+  </si>
+  <si>
+    <t>Prologue to Part II</t>
+  </si>
+  <si>
+    <t>PXPG2F62</t>
+  </si>
+  <si>
+    <t>P2PG1F63</t>
+  </si>
+  <si>
+    <t>Part II</t>
+  </si>
+  <si>
+    <t>P2PG2F64</t>
+  </si>
+  <si>
+    <t>P2PG3F65</t>
+  </si>
+  <si>
+    <t>P2PG4F65</t>
+  </si>
+  <si>
+    <t>P2PG5F66</t>
+  </si>
+  <si>
+    <t>P2PG6F67</t>
+  </si>
+  <si>
+    <t>P2PG7F68</t>
+  </si>
+  <si>
+    <t>P2PG8F69</t>
+  </si>
+  <si>
+    <t>P2PG9F70</t>
+  </si>
+  <si>
+    <t>P2PG10F71</t>
+  </si>
+  <si>
+    <t>P2PG11F72</t>
+  </si>
+  <si>
+    <t>P2PG12F73</t>
+  </si>
+  <si>
+    <t>P2PG13F74</t>
+  </si>
+  <si>
+    <t>P2PG14F75</t>
+  </si>
+  <si>
+    <t>P2PG15F76</t>
+  </si>
+  <si>
+    <t>P2PG16F77</t>
+  </si>
+  <si>
+    <t>P2PG17F78</t>
+  </si>
+  <si>
+    <t>P2PG18F79</t>
+  </si>
+  <si>
+    <t>P2PG19F80</t>
+  </si>
+  <si>
+    <t>P2PG20F81</t>
+  </si>
+  <si>
+    <t>Part II; interrupting marginalia; italic reference to plates</t>
+  </si>
+  <si>
+    <t>Part I; long margin comment</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Part I; interrupting marginalia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part I; large margin comment </t>
+  </si>
+  <si>
+    <t>Part II; italicized statnza (likely link to plate)</t>
+  </si>
+  <si>
+    <t>Part II; italicized stanza (link to plates)</t>
+  </si>
+  <si>
+    <t>Prologue to Rory Og confession monologue</t>
+  </si>
+  <si>
+    <t>PXPG1F82</t>
+  </si>
+  <si>
+    <t>PXPG2F83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rory Og confession narrative </t>
+  </si>
+  <si>
+    <t>P3PG1F84</t>
+  </si>
+  <si>
+    <t>P3PG2F85</t>
+  </si>
+  <si>
+    <t>P3PG3F86</t>
+  </si>
+  <si>
+    <t>P3PG4F87</t>
+  </si>
+  <si>
+    <t>P3PG5F88</t>
+  </si>
+  <si>
+    <t>P3PG6F89</t>
+  </si>
+  <si>
+    <t>P3PG7F90</t>
+  </si>
+  <si>
+    <t>P3PG8F91</t>
+  </si>
+  <si>
+    <t>P3PG9F92</t>
+  </si>
+  <si>
+    <t>P3PG10F93</t>
+  </si>
+  <si>
+    <t>P3PG11F94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rory Og confession narrative; interrupting marginalia  </t>
+  </si>
+  <si>
+    <t>PXPG1F95</t>
+  </si>
+  <si>
+    <t>PXPG2F96</t>
+  </si>
+  <si>
+    <t>PXPG3F97</t>
+  </si>
+  <si>
+    <t>P4PG1F98</t>
+  </si>
+  <si>
+    <t>P4PG2F99</t>
+  </si>
+  <si>
+    <t>P4PG3F100</t>
+  </si>
+  <si>
+    <t>P4PG4F101</t>
+  </si>
+  <si>
+    <t>P4PG5F102</t>
+  </si>
+  <si>
+    <t>PXPG1F103</t>
+  </si>
+  <si>
+    <t>Death of Rory Og</t>
+  </si>
+  <si>
+    <t>Prologue to Death of Rory Og</t>
+  </si>
+  <si>
+    <t>PXPG1F104</t>
+  </si>
+  <si>
+    <t>PXPG2F105</t>
+  </si>
+  <si>
+    <t>P5PG1F106</t>
+  </si>
+  <si>
+    <t>P5PG2F107</t>
+  </si>
+  <si>
+    <t>P5PG3F108</t>
+  </si>
+  <si>
+    <t>P5PG4F109</t>
+  </si>
+  <si>
+    <t>P5PG5F110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Death of Rory Og; pronounced "VV" opening section </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author's exhortation; sets up Rory Og in the woods  </t>
+  </si>
+  <si>
+    <t>http://www.docs.is.ed.ac.uk/docs/lib-archive/bgallery/Gallery/researchcoll/pages/bg0052_jpg.htm</t>
+  </si>
+  <si>
+    <t>Plate 1; handing a spear to an Irish lord</t>
+  </si>
+  <si>
+    <t>http://www.docs.is.ed.ac.uk/docs/lib-archive/bgallery/Gallery/researchcoll/pages/bg0053_jpg.htm</t>
+  </si>
+  <si>
+    <t>http://www.docs.is.ed.ac.uk/docs/lib-archive/bgallery/Gallery/researchcoll/pages/bg0054_jpg.htm</t>
+  </si>
+  <si>
+    <t>Plate 2; kerne setting house on fire; the Pale</t>
+  </si>
+  <si>
+    <t>http://www.docs.is.ed.ac.uk/docs/lib-archive/bgallery/Gallery/researchcoll/pages/bg0055_jpg.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plate 3; karnish dinner </t>
+  </si>
+  <si>
+    <t>http://www.docs.is.ed.ac.uk/docs/lib-archive/bgallery/Gallery/researchcoll/pages/bg0056_jpg.htm</t>
+  </si>
+  <si>
+    <t>Plate 4; battle; devilish friars on battlefield</t>
+  </si>
+  <si>
+    <t>http://www.docs.is.ed.ac.uk/docs/lib-archive/bgallery/Gallery/researchcoll/pages/bg0057_jpg.htm</t>
+  </si>
+  <si>
+    <t>Plate 5; English soldiers with kerne heads on swords</t>
+  </si>
+  <si>
+    <t>http://www.docs.is.ed.ac.uk/docs/lib-archive/bgallery/Gallery/researchcoll/pages/bg0058_jpg.htm</t>
+  </si>
+  <si>
+    <t>http://www.docs.is.ed.ac.uk/docs/lib-archive/bgallery/Gallery/researchcoll/pages/bg0059_jpg.htm</t>
+  </si>
+  <si>
+    <t>Plate 7; "shoph" messenger to Henry Sidney's camp</t>
+  </si>
+  <si>
+    <t>http://www.docs.is.ed.ac.uk/docs/lib-archive/bgallery/Gallery/researchcoll/pages/bg0060_jpg.htm</t>
+  </si>
+  <si>
+    <t>Plate 8; Henry Sidney marching with troops; pikes and horses</t>
+  </si>
+  <si>
+    <t>http://www.docs.is.ed.ac.uk/docs/lib-archive/bgallery/Gallery/researchcoll/pages/bg0061_jpg.htm</t>
+  </si>
+  <si>
+    <t>Plate 9; Irish and English fight; English winning; Irish piper stomped</t>
+  </si>
+  <si>
+    <t>http://www.docs.is.ed.ac.uk/docs/lib-archive/bgallery/Gallery/researchcoll/pages/bg0062_jpg.htm</t>
+  </si>
+  <si>
+    <t>Plate 10; Henry Sidney Dublin Castle; shaking hands after victory</t>
+  </si>
+  <si>
+    <t>Plate 6; Henry Sidney at Dublin Castle; heads on pikes above door</t>
+  </si>
+  <si>
+    <t>Plate 11; Rorie Og cloaked in the woods</t>
+  </si>
+  <si>
+    <t>http://www.docs.is.ed.ac.uk/docs/lib-archive/bgallery/Gallery/researchcoll/pages/bg0063_jpg.htm</t>
+  </si>
+  <si>
+    <t>http://www.docs.is.ed.ac.uk/docs/lib-archive/bgallery/Gallery/researchcoll/pages/bg0064_jpg.htm</t>
+  </si>
+  <si>
+    <t>Plate 12; O'Neal bows and submits to Henry Sidney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O'Neal submission; interrupting marginalia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O'Neal submission </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prologue to O'Neal submission </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rory Og confession narrative; large margin comment (full page) </t>
+  </si>
+  <si>
+    <t>Image of Phillip Sidney (1586); posthumously added</t>
   </si>
 </sst>
 </file>
@@ -978,16 +1230,19 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="73.6640625" customWidth="1"/>
+    <col min="4" max="4" width="87.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -997,8 +1252,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D1" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1006,812 +1264,1256 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A8" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A9" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D12" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D13" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D14" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A12" s="1" t="s">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A13" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D17" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A14" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="1" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A15" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="1" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A16" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="1" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A17" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A18" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A19" s="1" t="s">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A20" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C25" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A26" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C31" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A27" s="1" t="s">
+      <c r="C32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A33" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A28" s="1" t="s">
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A34" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A29" s="1" t="s">
+      <c r="C34" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A35" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A36" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A30" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A37" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A31" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A38" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A32" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A39" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A33" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C39" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A40" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A34" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A41" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A35" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A42" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A36" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A43" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A37" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A44" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A38" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A45" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A39" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A46" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A40" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A47" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A41" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A48" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A42" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A49" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A43" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A50" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A44" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A51" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A45" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A52" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A46" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C52" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A53" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A47" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="C53" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A54" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A48" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A55" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A49" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C55" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A56" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A50" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C56" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A57" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A51" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C57" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A58" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A52" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A59" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A53" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C59" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A60" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A54" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="C60" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A61" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A55" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A62" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A56" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="C62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A63" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A57" s="1" t="s">
+      <c r="B63" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C63" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A64" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B64" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C64" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A65" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A58" s="1" t="s">
+      <c r="B65" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C65" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A66" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B66" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C66" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A67" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A59" s="1" t="s">
+      <c r="B67" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C67" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A68" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B68" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C68" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A69" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A60" s="1" t="s">
+      <c r="B69" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C69" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A70" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B70" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C70" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A71" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A61" s="1" t="s">
+      <c r="B71" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C71" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A72" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B72" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C72" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A73" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A62" s="1" t="s">
+      <c r="B73" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C73" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A74" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B74" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C74" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A75" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A63" s="1" t="s">
+      <c r="B75" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C75" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A76" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A64" s="1" t="s">
+      <c r="B76" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C76" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A77" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A65" s="1" t="s">
+      <c r="B77" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C77" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A78" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A66" s="1" t="s">
+      <c r="B78" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C78" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A79" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A67" s="1" t="s">
+      <c r="B79" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C79" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A80" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A68" s="1" t="s">
+      <c r="B80" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C80" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A81" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A69" s="1" t="s">
+      <c r="B81" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C81" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A82" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A70" s="1" t="s">
+      <c r="B82" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C82" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A83" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A71" s="1" t="s">
+      <c r="B83" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C83" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A84" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A72" s="1" t="s">
+      <c r="B84" t="s">
+        <v>205</v>
+      </c>
+      <c r="C84" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A85" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A73" s="1" t="s">
+      <c r="B85" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C85" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A86" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A74" s="1" t="s">
+      <c r="B86" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C86" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A87" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A75" s="1" t="s">
+      <c r="B87" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C87" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A88" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A76" s="1" t="s">
+      <c r="B88" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C88" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A89" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A77" s="1" t="s">
+      <c r="B89" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C89" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A90" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A78" s="1" t="s">
+      <c r="B90" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C90" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A91" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A79" s="1" t="s">
+      <c r="B91" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C91" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A92" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A80" s="1" t="s">
+      <c r="B92" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C92" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A93" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A81" s="1" t="s">
+      <c r="B93" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C93" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A94" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A82" s="1" t="s">
+      <c r="B94" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C94" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A95" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A83" s="1" t="s">
+      <c r="B95" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C95" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A96" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A84" s="1" t="s">
+      <c r="B96" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C96" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A97" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A85" s="1" t="s">
+      <c r="B97" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C97" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A98" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A86" s="1" t="s">
+      <c r="B98" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C98" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A99" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A87" s="1" t="s">
+      <c r="B99" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C99" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A100" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A88" s="1" t="s">
+      <c r="B100" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C100" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A101" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A89" s="1" t="s">
+      <c r="B101" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C101" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A102" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A90" s="1" t="s">
+      <c r="B102" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C102" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A103" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A91" s="1" t="s">
+      <c r="B103" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C103" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A104" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A92" s="1" t="s">
+      <c r="B104" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C104" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A105" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A93" s="1" t="s">
+      <c r="B105" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C105" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A106" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A94" s="1" t="s">
+      <c r="B106" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C106" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A107" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A95" s="1" t="s">
+      <c r="B107" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C107" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A108" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A96" s="1" t="s">
+      <c r="B108" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C108" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A109" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A97" s="1" t="s">
+      <c r="B109" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C109" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A110" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A98" s="1" t="s">
+      <c r="B110" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C110" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A111" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A99" s="1" t="s">
+      <c r="B111" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C111" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A112" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A100" s="1" t="s">
+      <c r="B112" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C112" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A113" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A101" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A102" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A103" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A104" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A105" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A106" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A107" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A108" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A109" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A110" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A111" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A112" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A113" s="1" t="s">
-        <v>194</v>
+      <c r="B113" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C113" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>